<commit_message>
Add ASD and OS reports
</commit_message>
<xml_diff>
--- a/algorytmy i str danyh/labs zvits/Михалевич_ПЗ-23_ASD_lab7 (Recovered).xlsx
+++ b/algorytmy i str danyh/labs zvits/Михалевич_ПЗ-23_ASD_lab7 (Recovered).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Bubble</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Counting</t>
+  </si>
+  <si>
+    <t>Comparisons</t>
   </si>
 </sst>
 </file>
@@ -2119,7 +2122,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$1</c15:sqref>
@@ -2148,7 +2151,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$2:$A$8</c15:sqref>
@@ -2184,7 +2187,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$2:$C$8</c15:sqref>
@@ -2210,7 +2213,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-DB79-49CB-92E4-664BB3168B84}"/>
                   </c:ext>
@@ -2223,7 +2226,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$1</c15:sqref>
@@ -2252,7 +2255,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$2:$A$8</c15:sqref>
@@ -2288,7 +2291,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$2:$D$8</c15:sqref>
@@ -2323,7 +2326,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-DB79-49CB-92E4-664BB3168B84}"/>
                   </c:ext>
@@ -2967,7 +2970,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$1</c15:sqref>
@@ -2994,7 +2997,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$2:$A$8</c15:sqref>
@@ -3030,7 +3033,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$2:$C$8</c15:sqref>
@@ -3055,7 +3058,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-EF5B-4764-9ACB-E593C05FCB7E}"/>
                   </c:ext>
@@ -3068,7 +3071,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$1</c15:sqref>
@@ -3095,7 +3098,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$2:$A$8</c15:sqref>
@@ -3131,7 +3134,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$2:$D$8</c15:sqref>
@@ -3165,7 +3168,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-EF5B-4764-9ACB-E593C05FCB7E}"/>
                   </c:ext>
@@ -3322,6 +3325,738 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="uk-UA"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="uk-UA"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$32:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D91B-4726-A071-34F072D78E69}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Comparisons</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$32:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D91B-4726-A071-34F072D78E69}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="707883712"/>
+        <c:axId val="707884128"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="707883712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="707884128"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="707884128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="707883712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="uk-UA"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="uk-UA"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Comparisons</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$32:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$32:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DA91-406D-9D8F-492A799421FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="706966832"/>
+        <c:axId val="706968080"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="706966832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Size</a:t>
+                </a:r>
+                <a:endParaRPr lang="uk-UA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.45617935258092746"/>
+              <c:y val="0.87868037328667248"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="uk-UA"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="706968080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="706968080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Comparisons</a:t>
+                </a:r>
+                <a:endParaRPr lang="uk-UA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="uk-UA"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="706966832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3519,6 +4254,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -5204,6 +6019,1038 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5679,6 +7526,66 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5945,10 +7852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6116,6 +8023,43 @@
         <v>1600077</v>
       </c>
     </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>70</v>
+      </c>
+      <c r="B34">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>100</v>
+      </c>
+      <c r="B35">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>